<commit_message>
Add feature file and test cases  _Nikhil Xcel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAEDA83-AB9F-46A1-9B78-132F555576B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Admin</t>
   </si>
@@ -65,12 +66,21 @@
   </si>
   <si>
     <t>LoginPage:Manager;</t>
+  </si>
+  <si>
+    <t>MyInfo</t>
+  </si>
+  <si>
+    <t>Validate admin Section</t>
+  </si>
+  <si>
+    <t>Verify tab on Side Search bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,23 +429,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -452,7 +462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -466,6 +476,36 @@
         <v>14</v>
       </c>
       <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -474,20 +514,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -498,7 +538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -509,7 +549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>

</xml_diff>